<commit_message>
Localization for new dialogue in new scenarios set up. RoundNumber now set to 0 (random scenarios) if no SUGAR user is signed in.
</commit_message>
<xml_diff>
--- a/Assets/Editor/Localization/SMIScenarios.xlsx
+++ b/Assets/Editor/Localization/SMIScenarios.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="800">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="884">
   <si>
     <t>Key</t>
   </si>
@@ -2414,13 +2414,265 @@
   </si>
   <si>
     <t>But of course, just a moment...it's {0}.</t>
+  </si>
+  <si>
+    <t>Sterremotor type {0} doet het weer eens niet, waardeloos! Wat voor troep verkopen jullie eigenlijk?</t>
+  </si>
+  <si>
+    <t>Sensornet type {0} doet het weer eens niet, waardeloos! Wat voor troep verkopen jullie eigenlijk?</t>
+  </si>
+  <si>
+    <t>Krachtcel type {0} doet het weer eens niet, waardeloos! Wat voor troep verkopen jullie eigenlijk?</t>
+  </si>
+  <si>
+    <t>Wat is er aan de hand? Wat is er aan de hand?! Sterremotor type {0} is weer eens kapot, waardeloos is het!!</t>
+  </si>
+  <si>
+    <t>Wat is er aan de hand? Wat is er aan de hand?! Krachtcel type {0} is weer eens kapot, waardeloos is het!!</t>
+  </si>
+  <si>
+    <t>Wat is er aan de hand? Wat is er aan de hand?! Sensornet type {0} is weer eens kapot, waardeloos is het!!</t>
+  </si>
+  <si>
+    <t>The warp drive, type {0} has failed again, it's worthless! What kind of junk do you guys sell anyway?</t>
+  </si>
+  <si>
+    <t>The power cell, type {0} has failed again, it's worthless! What kind of junk do you guys sell anyway?</t>
+  </si>
+  <si>
+    <t>The sensor array, type {0} has failed again, it's worthless! What kind of junk do you guys sell anyway?</t>
+  </si>
+  <si>
+    <t>What's up? What's up?! The warp drive, type {0}, has failed once again!! It's worthless!</t>
+  </si>
+  <si>
+    <t>What's up? What's up?! The power cell, type {0}, has failed once again!! It's worthless!</t>
+  </si>
+  <si>
+    <t>What's up? What's up?! The sensor array, type {0}, has failed once again!! It's worthless!</t>
+  </si>
+  <si>
+    <t>Hi, I'm having trouble with the warp drive again. It's type {0}.</t>
+  </si>
+  <si>
+    <t>Hi, I'm having trouble with the power cell again. It's type {0}.</t>
+  </si>
+  <si>
+    <t>Hi, I'm having trouble with the sensor array again. It's type {0}.</t>
+  </si>
+  <si>
+    <t>Hee, ik heb weer eens problemen met Sterremotor, type {0}.</t>
+  </si>
+  <si>
+    <t>Hee, ik heb weer eens problemen met Krachtcel, type {0}.</t>
+  </si>
+  <si>
+    <t>Hee, ik heb weer eens problemen met Sensornet, type {0}.</t>
+  </si>
+  <si>
+    <t>Hi there, I'm having trouble with the warp drive. It's type {0}.</t>
+  </si>
+  <si>
+    <t>Hi there, I'm having trouble with the power cell. It's type {0}.</t>
+  </si>
+  <si>
+    <t>Hi there, I'm having trouble with the sensor array. It's type {0}.</t>
+  </si>
+  <si>
+    <t>Hoi hoi, ik heb problemen met Sterremotor, type {0}.</t>
+  </si>
+  <si>
+    <t>Hoi hoi, ik heb problemen met Krachtcel, type {0}.</t>
+  </si>
+  <si>
+    <t>Hoi hoi, ik heb problemen met Sensornet, type {0}.</t>
+  </si>
+  <si>
+    <t>A_OP1E_A_E1</t>
+  </si>
+  <si>
+    <t>A_OP1E_A_E2</t>
+  </si>
+  <si>
+    <t>A_OP1E_A_E3</t>
+  </si>
+  <si>
+    <t>A_OP1E_A_E4</t>
+  </si>
+  <si>
+    <t>A_OP1E_A_E5</t>
+  </si>
+  <si>
+    <t>A_OP1E_A_P1</t>
+  </si>
+  <si>
+    <t>A_OP1E_A_P2</t>
+  </si>
+  <si>
+    <t>A_OP1E_A_P3</t>
+  </si>
+  <si>
+    <t>A_OP1E_A_P4</t>
+  </si>
+  <si>
+    <t>A_OP1E_A_P5</t>
+  </si>
+  <si>
+    <t>A_OP1E_A_S1</t>
+  </si>
+  <si>
+    <t>A_OP1E_A_S2</t>
+  </si>
+  <si>
+    <t>A_OP1E_A_S3</t>
+  </si>
+  <si>
+    <t>A_OP1E_A_S4</t>
+  </si>
+  <si>
+    <t>A_OP1E_A_S5</t>
+  </si>
+  <si>
+    <t>A_OP2E_A_E1</t>
+  </si>
+  <si>
+    <t>A_OP2E_A_E2</t>
+  </si>
+  <si>
+    <t>A_OP2E_A_E3</t>
+  </si>
+  <si>
+    <t>A_OP2E_A_E4</t>
+  </si>
+  <si>
+    <t>A_OP2E_A_E5</t>
+  </si>
+  <si>
+    <t>A_OP2E_A_P1</t>
+  </si>
+  <si>
+    <t>A_OP2E_A_P2</t>
+  </si>
+  <si>
+    <t>A_OP2E_A_P3</t>
+  </si>
+  <si>
+    <t>A_OP2E_A_P4</t>
+  </si>
+  <si>
+    <t>A_OP2E_A_P5</t>
+  </si>
+  <si>
+    <t>A_OP2E_A_S1</t>
+  </si>
+  <si>
+    <t>A_OP2E_A_S2</t>
+  </si>
+  <si>
+    <t>A_OP2E_A_S3</t>
+  </si>
+  <si>
+    <t>A_OP2E_A_S4</t>
+  </si>
+  <si>
+    <t>A_OP2E_A_S5</t>
+  </si>
+  <si>
+    <t>A_OPE_N_E1</t>
+  </si>
+  <si>
+    <t>A_OPE_N_E2</t>
+  </si>
+  <si>
+    <t>A_OPE_N_E3</t>
+  </si>
+  <si>
+    <t>A_OPE_N_E4</t>
+  </si>
+  <si>
+    <t>A_OPE_N_E5</t>
+  </si>
+  <si>
+    <t>A_OPE_N_P1</t>
+  </si>
+  <si>
+    <t>A_OPE_N_P2</t>
+  </si>
+  <si>
+    <t>A_OPE_N_P3</t>
+  </si>
+  <si>
+    <t>A_OPE_N_P4</t>
+  </si>
+  <si>
+    <t>A_OPE_N_P5</t>
+  </si>
+  <si>
+    <t>A_OPE_N_S1</t>
+  </si>
+  <si>
+    <t>A_OPE_N_S2</t>
+  </si>
+  <si>
+    <t>A_OPE_N_S3</t>
+  </si>
+  <si>
+    <t>A_OPE_N_S4</t>
+  </si>
+  <si>
+    <t>A_OPE_N_S5</t>
+  </si>
+  <si>
+    <t>A_OPE_P_E1</t>
+  </si>
+  <si>
+    <t>A_OPE_P_E2</t>
+  </si>
+  <si>
+    <t>A_OPE_P_E3</t>
+  </si>
+  <si>
+    <t>A_OPE_P_E4</t>
+  </si>
+  <si>
+    <t>A_OPE_P_E5</t>
+  </si>
+  <si>
+    <t>A_OPE_P_P1</t>
+  </si>
+  <si>
+    <t>A_OPE_P_P2</t>
+  </si>
+  <si>
+    <t>A_OPE_P_P3</t>
+  </si>
+  <si>
+    <t>A_OPE_P_P4</t>
+  </si>
+  <si>
+    <t>A_OPE_P_P5</t>
+  </si>
+  <si>
+    <t>A_OPE_P_S1</t>
+  </si>
+  <si>
+    <t>A_OPE_P_S2</t>
+  </si>
+  <si>
+    <t>A_OPE_P_S3</t>
+  </si>
+  <si>
+    <t>A_OPE_P_S4</t>
+  </si>
+  <si>
+    <t>A_OPE_P_S5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2434,6 +2686,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -2464,7 +2722,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -2480,6 +2738,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2753,7 +3014,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2761,17 +3022,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C304"/>
+  <dimension ref="A1:C364"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B130" sqref="B130"/>
+      <pane ySplit="1" topLeftCell="A322" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B333" sqref="B333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" style="2" customWidth="1"/>
-    <col min="2" max="2" width="75.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="76.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="82.5703125" style="2" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" style="2" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" style="2" customWidth="1"/>
@@ -3203,7 +3464,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>379</v>
       </c>
@@ -4545,1591 +4806,2254 @@
         <v>331</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" s="3" t="s">
-        <v>429</v>
-      </c>
-      <c r="B161" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C161" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" s="3" t="s">
-        <v>430</v>
-      </c>
-      <c r="B162" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C162" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163" s="3" t="s">
-        <v>431</v>
-      </c>
-      <c r="B163" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C163" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A164" s="3" t="s">
-        <v>432</v>
-      </c>
-      <c r="B164" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C164" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A165" s="3" t="s">
-        <v>433</v>
-      </c>
-      <c r="B165" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C165" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A166" s="3" t="s">
-        <v>434</v>
-      </c>
-      <c r="B166" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C166" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167" s="3" t="s">
-        <v>435</v>
-      </c>
-      <c r="B167" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C167" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" s="3" t="s">
-        <v>436</v>
-      </c>
-      <c r="B168" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C168" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A169" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="B169" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C169" s="3" t="s">
-        <v>194</v>
+    <row r="161" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A161" s="6" t="s">
+        <v>824</v>
+      </c>
+      <c r="B161" s="6" t="s">
+        <v>806</v>
+      </c>
+      <c r="C161" s="6" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A162" s="2" t="s">
+        <v>825</v>
+      </c>
+      <c r="B162" s="6" t="s">
+        <v>806</v>
+      </c>
+      <c r="C162" s="6" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="s">
+        <v>826</v>
+      </c>
+      <c r="B163" s="6" t="s">
+        <v>806</v>
+      </c>
+      <c r="C163" s="6" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A164" s="2" t="s">
+        <v>827</v>
+      </c>
+      <c r="B164" s="6" t="s">
+        <v>806</v>
+      </c>
+      <c r="C164" s="6" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A165" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="B165" s="6" t="s">
+        <v>806</v>
+      </c>
+      <c r="C165" s="6" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A166" s="6" t="s">
+        <v>829</v>
+      </c>
+      <c r="B166" s="6" t="s">
+        <v>807</v>
+      </c>
+      <c r="C166" s="6" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A167" s="2" t="s">
+        <v>830</v>
+      </c>
+      <c r="B167" s="6" t="s">
+        <v>807</v>
+      </c>
+      <c r="C167" s="6" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A168" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="B168" s="6" t="s">
+        <v>807</v>
+      </c>
+      <c r="C168" s="6" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A169" s="2" t="s">
+        <v>832</v>
+      </c>
+      <c r="B169" s="6" t="s">
+        <v>807</v>
+      </c>
+      <c r="C169" s="6" t="s">
+        <v>802</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A170" s="3" t="s">
-        <v>438</v>
-      </c>
-      <c r="B170" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="C170" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A171" s="3" t="s">
-        <v>439</v>
-      </c>
-      <c r="B171" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C171" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172" s="3" t="s">
-        <v>440</v>
-      </c>
-      <c r="B172" s="3" t="s">
-        <v>725</v>
-      </c>
-      <c r="C172" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A173" s="3" t="s">
-        <v>441</v>
-      </c>
-      <c r="B173" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C173" s="3" t="s">
-        <v>198</v>
+      <c r="A170" s="2" t="s">
+        <v>833</v>
+      </c>
+      <c r="B170" s="6" t="s">
+        <v>807</v>
+      </c>
+      <c r="C170" s="6" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A171" s="6" t="s">
+        <v>834</v>
+      </c>
+      <c r="B171" s="6" t="s">
+        <v>808</v>
+      </c>
+      <c r="C171" s="6" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
+        <v>835</v>
+      </c>
+      <c r="B172" s="6" t="s">
+        <v>808</v>
+      </c>
+      <c r="C172" s="6" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A173" s="2" t="s">
+        <v>836</v>
+      </c>
+      <c r="B173" s="6" t="s">
+        <v>808</v>
+      </c>
+      <c r="C173" s="6" t="s">
+        <v>801</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A174" s="3" t="s">
-        <v>442</v>
-      </c>
-      <c r="B174" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C174" s="3" t="s">
-        <v>333</v>
+      <c r="A174" s="2" t="s">
+        <v>837</v>
+      </c>
+      <c r="B174" s="6" t="s">
+        <v>808</v>
+      </c>
+      <c r="C174" s="6" t="s">
+        <v>801</v>
       </c>
     </row>
     <row r="175" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A175" s="3" t="s">
-        <v>443</v>
-      </c>
-      <c r="B175" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C175" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A176" s="3" t="s">
-        <v>444</v>
-      </c>
-      <c r="B176" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C176" s="3" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A177" s="3" t="s">
-        <v>445</v>
-      </c>
-      <c r="B177" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C177" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A178" s="3" t="s">
-        <v>446</v>
-      </c>
-      <c r="B178" s="3" t="s">
-        <v>724</v>
-      </c>
-      <c r="C178" s="3" t="s">
-        <v>201</v>
+      <c r="A175" s="2" t="s">
+        <v>838</v>
+      </c>
+      <c r="B175" s="6" t="s">
+        <v>808</v>
+      </c>
+      <c r="C175" s="6" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A176" s="6" t="s">
+        <v>839</v>
+      </c>
+      <c r="B176" s="6" t="s">
+        <v>809</v>
+      </c>
+      <c r="C176" s="6" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A177" s="2" t="s">
+        <v>840</v>
+      </c>
+      <c r="B177" s="6" t="s">
+        <v>809</v>
+      </c>
+      <c r="C177" s="6" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A178" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="B178" s="6" t="s">
+        <v>809</v>
+      </c>
+      <c r="C178" s="6" t="s">
+        <v>803</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A179" s="3" t="s">
-        <v>447</v>
-      </c>
-      <c r="B179" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C179" s="3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A180" s="3" t="s">
-        <v>448</v>
-      </c>
-      <c r="B180" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C180" s="3" t="s">
-        <v>203</v>
+      <c r="A179" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="B179" s="6" t="s">
+        <v>809</v>
+      </c>
+      <c r="C179" s="6" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A180" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="B180" s="6" t="s">
+        <v>809</v>
+      </c>
+      <c r="C180" s="6" t="s">
+        <v>803</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A181" s="3" t="s">
-        <v>449</v>
-      </c>
-      <c r="B181" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C181" s="3" t="s">
-        <v>204</v>
+      <c r="A181" s="2" t="s">
+        <v>844</v>
+      </c>
+      <c r="B181" s="6" t="s">
+        <v>810</v>
+      </c>
+      <c r="C181" s="6" t="s">
+        <v>804</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A182" s="3" t="s">
-        <v>450</v>
-      </c>
-      <c r="B182" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C182" s="3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A183" s="3" t="s">
-        <v>451</v>
-      </c>
-      <c r="B183" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C183" s="3" t="s">
-        <v>206</v>
+      <c r="A182" s="2" t="s">
+        <v>845</v>
+      </c>
+      <c r="B182" s="6" t="s">
+        <v>810</v>
+      </c>
+      <c r="C182" s="6" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A183" s="2" t="s">
+        <v>846</v>
+      </c>
+      <c r="B183" s="6" t="s">
+        <v>810</v>
+      </c>
+      <c r="C183" s="6" t="s">
+        <v>804</v>
       </c>
     </row>
     <row r="184" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A184" s="3" t="s">
-        <v>452</v>
-      </c>
-      <c r="B184" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="C184" s="3" t="s">
-        <v>207</v>
+      <c r="A184" s="2" t="s">
+        <v>847</v>
+      </c>
+      <c r="B184" s="6" t="s">
+        <v>810</v>
+      </c>
+      <c r="C184" s="6" t="s">
+        <v>804</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A185" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="B185" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C185" s="3" t="s">
-        <v>208</v>
+      <c r="A185" s="2" t="s">
+        <v>848</v>
+      </c>
+      <c r="B185" s="6" t="s">
+        <v>810</v>
+      </c>
+      <c r="C185" s="6" t="s">
+        <v>804</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A186" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="B186" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C186" s="3" t="s">
-        <v>335</v>
+      <c r="A186" s="2" t="s">
+        <v>849</v>
+      </c>
+      <c r="B186" s="6" t="s">
+        <v>811</v>
+      </c>
+      <c r="C186" s="6" t="s">
+        <v>805</v>
       </c>
     </row>
     <row r="187" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A187" s="3" t="s">
-        <v>455</v>
-      </c>
-      <c r="B187" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C187" s="3" t="s">
-        <v>209</v>
+      <c r="A187" s="2" t="s">
+        <v>850</v>
+      </c>
+      <c r="B187" s="6" t="s">
+        <v>811</v>
+      </c>
+      <c r="C187" s="6" t="s">
+        <v>805</v>
       </c>
     </row>
     <row r="188" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A188" s="3" t="s">
-        <v>456</v>
-      </c>
-      <c r="B188" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C188" s="3" t="s">
-        <v>210</v>
+      <c r="A188" s="2" t="s">
+        <v>851</v>
+      </c>
+      <c r="B188" s="6" t="s">
+        <v>811</v>
+      </c>
+      <c r="C188" s="6" t="s">
+        <v>805</v>
       </c>
     </row>
     <row r="189" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A189" s="3" t="s">
-        <v>457</v>
-      </c>
-      <c r="B189" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C189" s="3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A190" s="3" t="s">
-        <v>458</v>
-      </c>
-      <c r="B190" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C190" s="3" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A191" s="3" t="s">
-        <v>459</v>
-      </c>
-      <c r="B191" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C191" s="3" t="s">
-        <v>212</v>
+      <c r="A189" s="2" t="s">
+        <v>852</v>
+      </c>
+      <c r="B189" s="6" t="s">
+        <v>811</v>
+      </c>
+      <c r="C189" s="6" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A190" s="2" t="s">
+        <v>853</v>
+      </c>
+      <c r="B190" s="6" t="s">
+        <v>811</v>
+      </c>
+      <c r="C190" s="6" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" s="2" t="s">
+        <v>854</v>
+      </c>
+      <c r="B191" s="6" t="s">
+        <v>812</v>
+      </c>
+      <c r="C191" s="6" t="s">
+        <v>815</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A192" s="3" t="s">
-        <v>460</v>
-      </c>
-      <c r="B192" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C192" s="3" t="s">
-        <v>213</v>
+      <c r="A192" s="2" t="s">
+        <v>855</v>
+      </c>
+      <c r="B192" s="6" t="s">
+        <v>812</v>
+      </c>
+      <c r="C192" s="6" t="s">
+        <v>815</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A193" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="B193" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C193" s="3" t="s">
-        <v>214</v>
+      <c r="A193" s="2" t="s">
+        <v>856</v>
+      </c>
+      <c r="B193" s="6" t="s">
+        <v>812</v>
+      </c>
+      <c r="C193" s="6" t="s">
+        <v>815</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A194" s="3" t="s">
-        <v>462</v>
-      </c>
-      <c r="B194" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="C194" s="3" t="s">
-        <v>215</v>
+      <c r="A194" s="2" t="s">
+        <v>857</v>
+      </c>
+      <c r="B194" s="6" t="s">
+        <v>812</v>
+      </c>
+      <c r="C194" s="6" t="s">
+        <v>815</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A195" s="3" t="s">
-        <v>463</v>
-      </c>
-      <c r="B195" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C195" s="3" t="s">
-        <v>216</v>
+      <c r="A195" s="2" t="s">
+        <v>858</v>
+      </c>
+      <c r="B195" s="6" t="s">
+        <v>812</v>
+      </c>
+      <c r="C195" s="6" t="s">
+        <v>815</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A196" s="3" t="s">
-        <v>464</v>
-      </c>
-      <c r="B196" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="C196" s="3" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A197" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="B197" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C197" s="3" t="s">
-        <v>218</v>
+      <c r="A196" s="2" t="s">
+        <v>859</v>
+      </c>
+      <c r="B196" s="6" t="s">
+        <v>813</v>
+      </c>
+      <c r="C196" s="6" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197" s="2" t="s">
+        <v>860</v>
+      </c>
+      <c r="B197" s="6" t="s">
+        <v>813</v>
+      </c>
+      <c r="C197" s="6" t="s">
+        <v>816</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A198" s="3" t="s">
-        <v>466</v>
-      </c>
-      <c r="B198" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C198" s="3" t="s">
-        <v>219</v>
+      <c r="A198" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="B198" s="6" t="s">
+        <v>813</v>
+      </c>
+      <c r="C198" s="6" t="s">
+        <v>816</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A199" s="3" t="s">
-        <v>467</v>
-      </c>
-      <c r="B199" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C199" s="3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A200" s="3" t="s">
-        <v>468</v>
-      </c>
-      <c r="B200" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C200" s="3" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A201" s="3" t="s">
-        <v>469</v>
-      </c>
-      <c r="B201" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="C201" s="3" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A202" s="3" t="s">
-        <v>470</v>
-      </c>
-      <c r="B202" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C202" s="3" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A203" s="3" t="s">
-        <v>471</v>
-      </c>
-      <c r="B203" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C203" s="3" t="s">
-        <v>223</v>
+      <c r="A199" s="2" t="s">
+        <v>862</v>
+      </c>
+      <c r="B199" s="6" t="s">
+        <v>813</v>
+      </c>
+      <c r="C199" s="6" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" s="2" t="s">
+        <v>863</v>
+      </c>
+      <c r="B200" s="6" t="s">
+        <v>813</v>
+      </c>
+      <c r="C200" s="6" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201" s="2" t="s">
+        <v>864</v>
+      </c>
+      <c r="B201" s="6" t="s">
+        <v>814</v>
+      </c>
+      <c r="C201" s="6" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202" s="2" t="s">
+        <v>865</v>
+      </c>
+      <c r="B202" s="6" t="s">
+        <v>814</v>
+      </c>
+      <c r="C202" s="6" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" s="2" t="s">
+        <v>866</v>
+      </c>
+      <c r="B203" s="6" t="s">
+        <v>814</v>
+      </c>
+      <c r="C203" s="6" t="s">
+        <v>817</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A204" s="3" t="s">
-        <v>472</v>
-      </c>
-      <c r="B204" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C204" s="3" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A205" s="3" t="s">
-        <v>473</v>
-      </c>
-      <c r="B205" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C205" s="3" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A206" s="3" t="s">
-        <v>474</v>
-      </c>
-      <c r="B206" s="4" t="s">
-        <v>723</v>
-      </c>
-      <c r="C206" s="3" t="s">
-        <v>226</v>
+      <c r="A204" s="2" t="s">
+        <v>867</v>
+      </c>
+      <c r="B204" s="6" t="s">
+        <v>814</v>
+      </c>
+      <c r="C204" s="6" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205" s="2" t="s">
+        <v>868</v>
+      </c>
+      <c r="B205" s="6" t="s">
+        <v>814</v>
+      </c>
+      <c r="C205" s="6" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206" s="6" t="s">
+        <v>869</v>
+      </c>
+      <c r="B206" s="6" t="s">
+        <v>818</v>
+      </c>
+      <c r="C206" s="6" t="s">
+        <v>821</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A207" s="3" t="s">
-        <v>475</v>
-      </c>
-      <c r="B207" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C207" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A208" s="3" t="s">
-        <v>476</v>
-      </c>
-      <c r="B208" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C208" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A209" s="3" t="s">
-        <v>477</v>
-      </c>
-      <c r="B209" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="C209" s="3" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A210" s="3" t="s">
-        <v>478</v>
-      </c>
-      <c r="B210" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C210" s="3" t="s">
-        <v>229</v>
+      <c r="A207" s="2" t="s">
+        <v>870</v>
+      </c>
+      <c r="B207" s="6" t="s">
+        <v>818</v>
+      </c>
+      <c r="C207" s="6" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" s="2" t="s">
+        <v>871</v>
+      </c>
+      <c r="B208" s="6" t="s">
+        <v>818</v>
+      </c>
+      <c r="C208" s="6" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" s="2" t="s">
+        <v>872</v>
+      </c>
+      <c r="B209" s="6" t="s">
+        <v>818</v>
+      </c>
+      <c r="C209" s="6" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" s="2" t="s">
+        <v>873</v>
+      </c>
+      <c r="B210" s="6" t="s">
+        <v>818</v>
+      </c>
+      <c r="C210" s="6" t="s">
+        <v>821</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A211" s="3" t="s">
-        <v>479</v>
-      </c>
-      <c r="B211" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C211" s="3" t="s">
-        <v>230</v>
+      <c r="A211" s="2" t="s">
+        <v>874</v>
+      </c>
+      <c r="B211" s="6" t="s">
+        <v>819</v>
+      </c>
+      <c r="C211" s="6" t="s">
+        <v>822</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A212" s="3" t="s">
-        <v>480</v>
-      </c>
-      <c r="B212" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C212" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A213" s="3" t="s">
-        <v>481</v>
-      </c>
-      <c r="B213" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C213" s="3" t="s">
-        <v>232</v>
+      <c r="A212" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="B212" s="6" t="s">
+        <v>819</v>
+      </c>
+      <c r="C212" s="6" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" s="2" t="s">
+        <v>876</v>
+      </c>
+      <c r="B213" s="6" t="s">
+        <v>819</v>
+      </c>
+      <c r="C213" s="6" t="s">
+        <v>822</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A214" s="3" t="s">
-        <v>482</v>
-      </c>
-      <c r="B214" s="4" t="s">
-        <v>336</v>
-      </c>
-      <c r="C214" s="3" t="s">
-        <v>233</v>
+      <c r="A214" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="B214" s="6" t="s">
+        <v>819</v>
+      </c>
+      <c r="C214" s="6" t="s">
+        <v>822</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A215" s="3" t="s">
-        <v>483</v>
-      </c>
-      <c r="B215" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="C215" s="3" t="s">
-        <v>234</v>
+      <c r="A215" s="2" t="s">
+        <v>878</v>
+      </c>
+      <c r="B215" s="6" t="s">
+        <v>819</v>
+      </c>
+      <c r="C215" s="6" t="s">
+        <v>822</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A216" s="3" t="s">
-        <v>484</v>
-      </c>
-      <c r="B216" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C216" s="3" t="s">
-        <v>235</v>
+      <c r="A216" s="2" t="s">
+        <v>879</v>
+      </c>
+      <c r="B216" s="6" t="s">
+        <v>820</v>
+      </c>
+      <c r="C216" s="6" t="s">
+        <v>823</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A217" s="3" t="s">
-        <v>485</v>
-      </c>
-      <c r="B217" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C217" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A218" s="3" t="s">
-        <v>486</v>
-      </c>
-      <c r="B218" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C218" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A219" s="3" t="s">
-        <v>487</v>
-      </c>
-      <c r="B219" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C219" s="3" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A220" s="3" t="s">
-        <v>488</v>
-      </c>
-      <c r="B220" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C220" s="3" t="s">
-        <v>238</v>
+      <c r="A217" s="2" t="s">
+        <v>880</v>
+      </c>
+      <c r="B217" s="6" t="s">
+        <v>820</v>
+      </c>
+      <c r="C217" s="6" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218" s="2" t="s">
+        <v>881</v>
+      </c>
+      <c r="B218" s="6" t="s">
+        <v>820</v>
+      </c>
+      <c r="C218" s="6" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219" s="2" t="s">
+        <v>882</v>
+      </c>
+      <c r="B219" s="6" t="s">
+        <v>820</v>
+      </c>
+      <c r="C219" s="6" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220" s="2" t="s">
+        <v>883</v>
+      </c>
+      <c r="B220" s="6" t="s">
+        <v>820</v>
+      </c>
+      <c r="C220" s="6" t="s">
+        <v>823</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
-        <v>489</v>
+        <v>524</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>337</v>
+        <v>117</v>
       </c>
       <c r="C221" s="3" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="3" t="s">
-        <v>490</v>
+        <v>549</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>338</v>
+        <v>612</v>
       </c>
       <c r="C222" s="3" t="s">
-        <v>239</v>
+        <v>659</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="3" t="s">
-        <v>491</v>
-      </c>
-      <c r="B223" s="4" t="s">
-        <v>97</v>
+        <v>558</v>
+      </c>
+      <c r="B223" s="3" t="s">
+        <v>629</v>
       </c>
       <c r="C223" s="3" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="224" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="s">
-        <v>492</v>
+        <v>550</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>98</v>
+        <v>613</v>
       </c>
       <c r="C224" s="3" t="s">
-        <v>241</v>
+        <v>658</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
-        <v>493</v>
+        <v>551</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>99</v>
+        <v>614</v>
       </c>
       <c r="C225" s="3" t="s">
-        <v>242</v>
+        <v>657</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="3" t="s">
-        <v>494</v>
+        <v>552</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>100</v>
+        <v>635</v>
       </c>
       <c r="C226" s="3" t="s">
-        <v>243</v>
+        <v>656</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
-        <v>495</v>
+        <v>553</v>
       </c>
       <c r="B227" s="3" t="s">
-        <v>322</v>
+        <v>634</v>
       </c>
       <c r="C227" s="3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="3" t="s">
-        <v>496</v>
+        <v>554</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>101</v>
+        <v>633</v>
       </c>
       <c r="C228" s="3" t="s">
-        <v>245</v>
+        <v>654</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="s">
-        <v>497</v>
+        <v>555</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>102</v>
+        <v>632</v>
       </c>
       <c r="C229" s="3" t="s">
-        <v>246</v>
+        <v>653</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="s">
-        <v>498</v>
+        <v>556</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>103</v>
+        <v>631</v>
       </c>
       <c r="C230" s="3" t="s">
-        <v>247</v>
+        <v>652</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="3" t="s">
-        <v>499</v>
+        <v>557</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>104</v>
+        <v>630</v>
       </c>
       <c r="C231" s="3" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="232" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="3" t="s">
-        <v>500</v>
+        <v>509</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>339</v>
+        <v>109</v>
       </c>
       <c r="C232" s="3" t="s">
-        <v>340</v>
+        <v>252</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="3" t="s">
-        <v>501</v>
+        <v>511</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C233" s="3" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" s="3" t="s">
-        <v>502</v>
+        <v>519</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>722</v>
+        <v>112</v>
       </c>
       <c r="C234" s="3" t="s">
-        <v>341</v>
+        <v>255</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="3" t="s">
-        <v>503</v>
+        <v>520</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="C235" s="3" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" s="3" t="s">
-        <v>504</v>
+        <v>521</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C236" s="3" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A237" s="3" t="s">
-        <v>505</v>
+        <v>522</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="C237" s="3" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A238" s="3" t="s">
-        <v>506</v>
+        <v>523</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>716</v>
+        <v>116</v>
       </c>
       <c r="C238" s="3" t="s">
-        <v>719</v>
+        <v>284</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" s="3" t="s">
-        <v>507</v>
+        <v>565</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>717</v>
+        <v>622</v>
       </c>
       <c r="C239" s="3" t="s">
-        <v>720</v>
+        <v>643</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" s="3" t="s">
-        <v>508</v>
+        <v>566</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>718</v>
+        <v>621</v>
       </c>
       <c r="C240" s="3" t="s">
-        <v>721</v>
+        <v>642</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" s="3" t="s">
-        <v>509</v>
+        <v>567</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>109</v>
+        <v>620</v>
       </c>
       <c r="C241" s="3" t="s">
-        <v>252</v>
+        <v>641</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" s="3" t="s">
-        <v>510</v>
+        <v>568</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>110</v>
+        <v>619</v>
       </c>
       <c r="C242" s="3" t="s">
-        <v>253</v>
+        <v>640</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" s="3" t="s">
-        <v>511</v>
+        <v>569</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>111</v>
+        <v>618</v>
       </c>
       <c r="C243" s="3" t="s">
-        <v>254</v>
+        <v>639</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" s="3" t="s">
-        <v>512</v>
+        <v>570</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>579</v>
+        <v>617</v>
       </c>
       <c r="C244" s="3" t="s">
-        <v>580</v>
+        <v>638</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" s="3" t="s">
-        <v>513</v>
+        <v>571</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>582</v>
+        <v>616</v>
       </c>
       <c r="C245" s="3" t="s">
-        <v>581</v>
+        <v>637</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" s="3" t="s">
-        <v>514</v>
+        <v>572</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>583</v>
+        <v>615</v>
       </c>
       <c r="C246" s="3" t="s">
-        <v>688</v>
+        <v>636</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" s="3" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="C247" s="3" t="s">
-        <v>687</v>
+        <v>580</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" s="3" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="C248" s="3" t="s">
-        <v>686</v>
+        <v>581</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" s="3" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="C249" s="3" t="s">
-        <v>685</v>
+        <v>688</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" s="3" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="C250" s="3" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" s="3" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>112</v>
+        <v>586</v>
       </c>
       <c r="C251" s="3" t="s">
-        <v>255</v>
+        <v>685</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" s="3" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>113</v>
+        <v>587</v>
       </c>
       <c r="C252" s="3" t="s">
-        <v>256</v>
+        <v>684</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" s="3" t="s">
-        <v>521</v>
+        <v>537</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>114</v>
+        <v>598</v>
       </c>
       <c r="C253" s="3" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="254" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" s="3" t="s">
-        <v>522</v>
+        <v>538</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>115</v>
+        <v>599</v>
       </c>
       <c r="C254" s="3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="255" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" s="3" t="s">
-        <v>523</v>
+        <v>539</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>116</v>
+        <v>600</v>
       </c>
       <c r="C255" s="3" t="s">
-        <v>284</v>
+        <v>669</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" s="3" t="s">
-        <v>524</v>
+        <v>540</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>117</v>
+        <v>601</v>
       </c>
       <c r="C256" s="3" t="s">
-        <v>259</v>
+        <v>668</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" s="3" t="s">
-        <v>525</v>
+        <v>541</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>588</v>
+        <v>602</v>
       </c>
       <c r="C257" s="3" t="s">
-        <v>683</v>
+        <v>667</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" s="3" t="s">
-        <v>526</v>
+        <v>542</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>589</v>
+        <v>605</v>
       </c>
       <c r="C258" s="3" t="s">
-        <v>682</v>
+        <v>666</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" s="3" t="s">
-        <v>527</v>
+        <v>559</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>590</v>
+        <v>628</v>
       </c>
       <c r="C259" s="3" t="s">
-        <v>681</v>
+        <v>649</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" s="3" t="s">
-        <v>528</v>
+        <v>560</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>591</v>
+        <v>627</v>
       </c>
       <c r="C260" s="3" t="s">
-        <v>680</v>
+        <v>648</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" s="3" t="s">
-        <v>529</v>
+        <v>561</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>592</v>
+        <v>626</v>
       </c>
       <c r="C261" s="3" t="s">
-        <v>679</v>
+        <v>647</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" s="3" t="s">
-        <v>530</v>
+        <v>562</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>593</v>
+        <v>625</v>
       </c>
       <c r="C262" s="3" t="s">
-        <v>678</v>
+        <v>646</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" s="3" t="s">
-        <v>531</v>
-      </c>
-      <c r="B263" s="3" t="s">
-        <v>594</v>
+        <v>563</v>
+      </c>
+      <c r="B263" s="5" t="s">
+        <v>624</v>
       </c>
       <c r="C263" s="3" t="s">
-        <v>677</v>
+        <v>645</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" s="3" t="s">
-        <v>532</v>
+        <v>564</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>595</v>
+        <v>623</v>
       </c>
       <c r="C264" s="3" t="s">
-        <v>676</v>
+        <v>644</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" s="3" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
       <c r="C265" s="3" t="s">
-        <v>675</v>
+        <v>683</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" s="3" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
       <c r="C266" s="3" t="s">
-        <v>674</v>
+        <v>682</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" s="3" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>603</v>
+        <v>590</v>
       </c>
       <c r="C267" s="3" t="s">
-        <v>673</v>
+        <v>681</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" s="3" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="C268" s="3" t="s">
-        <v>672</v>
+        <v>680</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" s="3" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
       <c r="C269" s="3" t="s">
-        <v>671</v>
+        <v>679</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" s="3" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="C270" s="3" t="s">
-        <v>670</v>
+        <v>678</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" s="3" t="s">
-        <v>539</v>
+        <v>543</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>600</v>
+        <v>606</v>
       </c>
       <c r="C271" s="3" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" s="3" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>601</v>
+        <v>607</v>
       </c>
       <c r="C272" s="3" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" s="3" t="s">
-        <v>541</v>
+        <v>545</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>602</v>
+        <v>608</v>
       </c>
       <c r="C273" s="3" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" s="3" t="s">
-        <v>542</v>
+        <v>546</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>605</v>
+        <v>609</v>
       </c>
       <c r="C274" s="3" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" s="3" t="s">
-        <v>543</v>
+        <v>547</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>606</v>
+        <v>610</v>
       </c>
       <c r="C275" s="3" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" s="3" t="s">
-        <v>544</v>
+        <v>548</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>607</v>
+        <v>611</v>
       </c>
       <c r="C276" s="3" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" s="3" t="s">
-        <v>545</v>
+        <v>510</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>608</v>
+        <v>110</v>
       </c>
       <c r="C277" s="3" t="s">
-        <v>663</v>
+        <v>253</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" s="3" t="s">
-        <v>546</v>
+        <v>531</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>609</v>
+        <v>594</v>
       </c>
       <c r="C278" s="3" t="s">
-        <v>662</v>
+        <v>677</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" s="3" t="s">
-        <v>547</v>
+        <v>532</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>610</v>
+        <v>595</v>
       </c>
       <c r="C279" s="3" t="s">
-        <v>661</v>
+        <v>676</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" s="3" t="s">
-        <v>548</v>
+        <v>533</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>611</v>
+        <v>596</v>
       </c>
       <c r="C280" s="3" t="s">
-        <v>660</v>
+        <v>675</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" s="3" t="s">
-        <v>549</v>
+        <v>534</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>612</v>
+        <v>597</v>
       </c>
       <c r="C281" s="3" t="s">
-        <v>659</v>
+        <v>674</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" s="3" t="s">
-        <v>550</v>
+        <v>535</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>613</v>
+        <v>603</v>
       </c>
       <c r="C282" s="3" t="s">
-        <v>658</v>
+        <v>673</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283" s="3" t="s">
-        <v>551</v>
+        <v>536</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>614</v>
+        <v>604</v>
       </c>
       <c r="C283" s="3" t="s">
-        <v>657</v>
+        <v>672</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" s="3" t="s">
-        <v>552</v>
+        <v>515</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>635</v>
+        <v>584</v>
       </c>
       <c r="C284" s="3" t="s">
-        <v>656</v>
+        <v>687</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" s="3" t="s">
-        <v>553</v>
+        <v>429</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>634</v>
+        <v>48</v>
       </c>
       <c r="C285" s="3" t="s">
-        <v>655</v>
+        <v>186</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" s="3" t="s">
-        <v>554</v>
+        <v>430</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>633</v>
+        <v>49</v>
       </c>
       <c r="C286" s="3" t="s">
-        <v>654</v>
+        <v>187</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" s="3" t="s">
-        <v>555</v>
+        <v>431</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>632</v>
+        <v>50</v>
       </c>
       <c r="C287" s="3" t="s">
-        <v>653</v>
+        <v>188</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" s="3" t="s">
-        <v>556</v>
+        <v>432</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>631</v>
+        <v>51</v>
       </c>
       <c r="C288" s="3" t="s">
-        <v>652</v>
+        <v>189</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" s="3" t="s">
-        <v>557</v>
+        <v>433</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>630</v>
+        <v>52</v>
       </c>
       <c r="C289" s="3" t="s">
-        <v>651</v>
+        <v>190</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" s="3" t="s">
-        <v>558</v>
+        <v>434</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>629</v>
+        <v>53</v>
       </c>
       <c r="C290" s="3" t="s">
-        <v>650</v>
+        <v>191</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" s="3" t="s">
-        <v>559</v>
+        <v>435</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>628</v>
+        <v>54</v>
       </c>
       <c r="C291" s="3" t="s">
-        <v>649</v>
+        <v>192</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" s="3" t="s">
-        <v>560</v>
+        <v>436</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>627</v>
+        <v>55</v>
       </c>
       <c r="C292" s="3" t="s">
-        <v>648</v>
+        <v>193</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" s="3" t="s">
-        <v>561</v>
+        <v>437</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>626</v>
+        <v>56</v>
       </c>
       <c r="C293" s="3" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A294" s="3" t="s">
-        <v>562</v>
+        <v>438</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>625</v>
+        <v>332</v>
       </c>
       <c r="C294" s="3" t="s">
-        <v>646</v>
+        <v>195</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" s="3" t="s">
-        <v>563</v>
-      </c>
-      <c r="B295" s="5" t="s">
-        <v>624</v>
+        <v>439</v>
+      </c>
+      <c r="B295" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="C295" s="3" t="s">
-        <v>645</v>
+        <v>196</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" s="3" t="s">
-        <v>564</v>
+        <v>440</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>623</v>
+        <v>725</v>
       </c>
       <c r="C296" s="3" t="s">
-        <v>644</v>
+        <v>197</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" s="3" t="s">
-        <v>565</v>
+        <v>441</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>622</v>
+        <v>58</v>
       </c>
       <c r="C297" s="3" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A298" s="3" t="s">
-        <v>566</v>
+        <v>442</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>621</v>
+        <v>59</v>
       </c>
       <c r="C298" s="3" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A299" s="3" t="s">
-        <v>567</v>
+        <v>443</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>620</v>
+        <v>60</v>
       </c>
       <c r="C299" s="3" t="s">
-        <v>641</v>
+        <v>199</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300" s="3" t="s">
-        <v>568</v>
+        <v>444</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>619</v>
+        <v>61</v>
       </c>
       <c r="C300" s="3" t="s">
-        <v>640</v>
+        <v>334</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" s="3" t="s">
-        <v>569</v>
+        <v>445</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>618</v>
+        <v>62</v>
       </c>
       <c r="C301" s="3" t="s">
-        <v>639</v>
+        <v>200</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" s="3" t="s">
-        <v>570</v>
+        <v>446</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>617</v>
+        <v>724</v>
       </c>
       <c r="C302" s="3" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A303" s="3" t="s">
-        <v>571</v>
+        <v>447</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>616</v>
+        <v>63</v>
       </c>
       <c r="C303" s="3" t="s">
-        <v>637</v>
+        <v>202</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A304" s="3" t="s">
-        <v>572</v>
+        <v>448</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>615</v>
+        <v>64</v>
       </c>
       <c r="C304" s="3" t="s">
-        <v>636</v>
+        <v>203</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A305" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="B305" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C305" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A306" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="B306" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C306" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A307" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="B307" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C307" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A308" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="B308" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="C308" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A309" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="B309" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C309" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A310" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="B310" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C310" s="3" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A311" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="B311" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C311" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A312" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="B312" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C312" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A313" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="B313" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C313" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A314" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="B314" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C314" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A315" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="B315" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C315" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A316" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="B316" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C316" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A317" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B317" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C317" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A318" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="B318" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C318" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A319" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="B319" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C319" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A320" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="B320" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="C320" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A321" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B321" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C321" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A322" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="B322" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C322" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A323" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="B323" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C323" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A324" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="B324" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C324" s="3" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A325" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="B325" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="C325" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A326" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="B326" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C326" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A327" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="B327" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C327" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A328" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="B328" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C328" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A329" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="B329" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C329" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A330" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="B330" s="4" t="s">
+        <v>723</v>
+      </c>
+      <c r="C330" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A331" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="B331" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C331" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A332" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="B332" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C332" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A333" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="B333" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C333" s="3" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A334" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="B334" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C334" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A335" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="B335" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C335" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A336" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="B336" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C336" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A337" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="B337" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C337" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A338" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="B338" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="C338" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A339" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="B339" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C339" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A340" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="B340" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C340" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A341" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="B341" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C341" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="342" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A342" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="B342" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C342" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="343" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A343" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="B343" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C343" s="3" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A344" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="B344" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C344" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A345" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="B345" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="C345" s="3" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A346" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="B346" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="C346" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A347" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="B347" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C347" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="348" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A348" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="B348" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C348" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A349" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="B349" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C349" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A350" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="B350" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C350" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A351" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="B351" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C351" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="352" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A352" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="B352" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C352" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A353" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="B353" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C353" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A354" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="B354" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C354" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A355" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="B355" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C355" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="356" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A356" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="B356" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="C356" s="3" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A357" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="B357" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C357" s="3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A358" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="B358" s="3" t="s">
+        <v>722</v>
+      </c>
+      <c r="C358" s="3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A359" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="B359" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C359" s="3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="360" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A360" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="B360" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C360" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A361" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="B361" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C361" s="3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A362" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="B362" s="3" t="s">
+        <v>716</v>
+      </c>
+      <c r="C362" s="3" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="363" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A363" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="B363" s="3" t="s">
+        <v>717</v>
+      </c>
+      <c r="C363" s="3" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="364" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A364" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="B364" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="C364" s="3" t="s">
+        <v>721</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:C364">
+    <sortCondition ref="A364"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>